<commit_message>
1. add print date info
</commit_message>
<xml_diff>
--- a/质量数据.xlsx
+++ b/质量数据.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>9月第3周</t>
   </si>
@@ -124,18 +124,18 @@
     <t>TOP 2</t>
   </si>
   <si>
+    <t>2.12.3-etm|6</t>
+  </si>
+  <si>
+    <t>2.16.3-tgp-plugin|6</t>
+  </si>
+  <si>
+    <t>TOP 3</t>
+  </si>
+  <si>
     <t>2.12.3-rule_mgr|11</t>
   </si>
   <si>
-    <t>2.16.3-tgp-plugin|6</t>
-  </si>
-  <si>
-    <t>TOP 3</t>
-  </si>
-  <si>
-    <t>2.12.3-etm|6</t>
-  </si>
-  <si>
     <t>2.16.3-etm|11</t>
   </si>
   <si>
@@ -145,18 +145,18 @@
     <t>2.12.3-sysapihttpd|6</t>
   </si>
   <si>
+    <t>2.16.3-cachecenter|11</t>
+  </si>
+  <si>
+    <t>TOP 5</t>
+  </si>
+  <si>
+    <t>2.12.3-etm|11</t>
+  </si>
+  <si>
     <t>2.16.3-indexservice|6</t>
   </si>
   <si>
-    <t>TOP 5</t>
-  </si>
-  <si>
-    <t>2.12.3-etm|11</t>
-  </si>
-  <si>
-    <t>2.16.3-cachecenter|11</t>
-  </si>
-  <si>
     <t>TOP 6</t>
   </si>
   <si>
@@ -181,24 +181,24 @@
     <t>2.12.3-iqiyi_server|11</t>
   </si>
   <si>
+    <t>2.16.3-thread_pool|11</t>
+  </si>
+  <si>
+    <t>TOP 9</t>
+  </si>
+  <si>
+    <t>2.12.3-smbd|10</t>
+  </si>
+  <si>
     <t>2.16.3-P2PEngine|11</t>
   </si>
   <si>
-    <t>TOP 9</t>
+    <t>TOP 10</t>
   </si>
   <si>
     <t>2.12.3-iqiyi_server|10</t>
   </si>
   <si>
-    <t>2.16.3-thread_pool|11</t>
-  </si>
-  <si>
-    <t>TOP 10</t>
-  </si>
-  <si>
-    <t>2.12.3-smbd|10</t>
-  </si>
-  <si>
     <t>2.16.3-etm|6</t>
   </si>
   <si>
@@ -223,19 +223,16 @@
     <t>2.14.6-taskmonitorServ|4</t>
   </si>
   <si>
+    <t>2.16.3-iqiyi_server|6</t>
+  </si>
+  <si>
+    <t>2.14.6-taskmonitorServ|11</t>
+  </si>
+  <si>
     <t>2.14.6-iwevent-call|11</t>
   </si>
   <si>
-    <t>2.16.3-iqiyi_server|6</t>
-  </si>
-  <si>
     <t>2.14.6-awk|11</t>
-  </si>
-  <si>
-    <t>2.16.3-tunnelserver|11</t>
-  </si>
-  <si>
-    <t>2.14.6-taskmonitorServ|11</t>
   </si>
 </sst>
 </file>
@@ -758,7 +755,7 @@
         <v>1088</v>
       </c>
       <c s="4" r="E3" t="n">
-        <v>2957</v>
+        <v>2932</v>
       </c>
       <c s="5" r="F3">
         <f si="0" ref="F3:F6" t="shared">(E3-D3)/D3</f>
@@ -774,7 +771,7 @@
         <v>671</v>
       </c>
       <c s="4" r="E4" t="n">
-        <v>1245</v>
+        <v>1218</v>
       </c>
       <c s="5" r="F4">
         <f si="0" t="shared"/>
@@ -790,7 +787,7 @@
         <v>2219864</v>
       </c>
       <c s="4" r="E5" t="n">
-        <v>2221863</v>
+        <v>2222199</v>
       </c>
       <c s="5" r="F5">
         <f si="0" t="shared"/>
@@ -807,7 +804,7 @@
         <v/>
       </c>
       <c s="5" r="E6" t="n">
-        <v>0.99944</v>
+        <v>0.9994499999999999</v>
       </c>
       <c s="5" r="F6">
         <f si="0" t="shared"/>
@@ -858,7 +855,7 @@
         <v>272130</v>
       </c>
       <c s="4" r="E9" t="n">
-        <v>271775</v>
+        <v>271681</v>
       </c>
       <c s="5" r="F9">
         <f si="1" t="shared"/>
@@ -902,7 +899,7 @@
         <v>510</v>
       </c>
       <c s="4" r="E11" t="n">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c s="5" r="F11">
         <f si="2" ref="F11:F14" t="shared">(E11-D11)/D11</f>
@@ -919,7 +916,7 @@
         <v>414</v>
       </c>
       <c s="4" r="E12" t="n">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c s="5" r="F12">
         <f si="2" t="shared"/>
@@ -936,7 +933,7 @@
         <v>163068</v>
       </c>
       <c s="4" r="E13" t="n">
-        <v>164085</v>
+        <v>164137</v>
       </c>
       <c s="5" r="F13">
         <f si="2" t="shared"/>
@@ -974,7 +971,7 @@
         <v>412</v>
       </c>
       <c s="4" r="E15" t="n">
-        <v>543</v>
+        <v>517</v>
       </c>
       <c s="5" r="F15">
         <f si="3" ref="F15:F18" t="shared">(E15-D15)/D15</f>
@@ -991,7 +988,7 @@
         <v>362</v>
       </c>
       <c s="4" r="E16" t="n">
-        <v>495</v>
+        <v>469</v>
       </c>
       <c s="5" r="F16">
         <f si="3" t="shared"/>
@@ -1008,7 +1005,7 @@
         <v>467469</v>
       </c>
       <c s="4" r="E17" t="n">
-        <v>476433</v>
+        <v>476464</v>
       </c>
       <c s="5" r="F17">
         <f si="3" t="shared"/>
@@ -1025,7 +1022,7 @@
         <v/>
       </c>
       <c s="5" r="E18" t="n">
-        <v>0.99896</v>
+        <v>0.99902</v>
       </c>
       <c s="5" r="F18">
         <f si="3" t="shared"/>
@@ -1043,7 +1040,7 @@
         <v>451</v>
       </c>
       <c s="4" r="E19" t="n">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c s="5" r="F19">
         <f si="4" ref="F19:F22" t="shared">(E19-D19)/D19</f>
@@ -1058,7 +1055,7 @@
         <v>320</v>
       </c>
       <c s="4" r="E20" t="n">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c s="5" r="F20">
         <f si="4" t="shared"/>
@@ -1073,7 +1070,7 @@
         <v>726568</v>
       </c>
       <c s="4" r="E21" t="n">
-        <v>753239</v>
+        <v>755470</v>
       </c>
       <c s="5" r="F21">
         <f si="4" t="shared"/>
@@ -1108,7 +1105,7 @@
         <v>2</v>
       </c>
       <c s="4" r="E23" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c s="5" r="F23">
         <f si="5" ref="F23:F26" t="shared">(E23-D23)/D23</f>
@@ -1140,7 +1137,7 @@
         <v>79058</v>
       </c>
       <c s="4" r="E25" t="n">
-        <v>91143</v>
+        <v>92033</v>
       </c>
       <c s="5" r="F25">
         <f si="5" t="shared"/>
@@ -1176,7 +1173,7 @@
         <v>799</v>
       </c>
       <c s="4" r="E27" t="n">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c s="5" r="F27">
         <f si="6" ref="F27:F30" t="shared">(E27-D27)/D27</f>
@@ -1192,7 +1189,7 @@
         <v>579</v>
       </c>
       <c s="4" r="E28" t="n">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c s="5" r="F28">
         <f si="6" t="shared"/>
@@ -1208,7 +1205,7 @@
         <v>227185</v>
       </c>
       <c s="4" r="E29" t="n">
-        <v>235762</v>
+        <v>241475</v>
       </c>
       <c s="5" r="F29">
         <f si="6" t="shared"/>
@@ -1225,7 +1222,7 @@
         <v/>
       </c>
       <c s="5" r="E30" t="n">
-        <v>0.99754</v>
+        <v>0.99762</v>
       </c>
       <c s="5" r="F30">
         <f si="6" t="shared"/>
@@ -1244,7 +1241,7 @@
         <v>401</v>
       </c>
       <c s="4" r="E31" t="n">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c s="5" r="F31">
         <f si="7" ref="F31:F34" t="shared">(E31-D31)/D31</f>
@@ -1260,7 +1257,7 @@
         <v>334</v>
       </c>
       <c s="4" r="E32" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c s="5" r="F32">
         <f si="7" t="shared"/>
@@ -1276,7 +1273,7 @@
         <v>126798</v>
       </c>
       <c s="4" r="E33" t="n">
-        <v>131792</v>
+        <v>134608</v>
       </c>
       <c s="5" r="F33">
         <f si="7" t="shared"/>
@@ -1293,7 +1290,7 @@
         <v/>
       </c>
       <c s="5" r="E34" t="n">
-        <v>0.99732</v>
+        <v>0.99738</v>
       </c>
       <c s="5" r="F34">
         <f si="7" t="shared"/>
@@ -2310,7 +2307,7 @@
         <v>1.8</v>
       </c>
       <c s="4" r="E4" t="n">
-        <v>2039</v>
+        <v>2014</v>
       </c>
       <c s="5" r="F4" t="n"/>
     </row>
@@ -2322,7 +2319,7 @@
         <v>2</v>
       </c>
       <c s="4" r="E5" t="n">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c s="5" r="F5" t="n"/>
     </row>
@@ -2334,7 +2331,7 @@
         <v>1208033</v>
       </c>
       <c s="4" r="E6" t="n">
-        <v>583233</v>
+        <v>666466</v>
       </c>
       <c s="5" r="F6" t="n"/>
     </row>
@@ -2346,7 +2343,7 @@
         <v>0.99999</v>
       </c>
       <c s="5" r="E7" t="n">
-        <v>0.99903</v>
+        <v>0.99917</v>
       </c>
       <c s="5" r="F7">
         <f>(E7-D7)/D7</f>
@@ -2400,7 +2397,7 @@
         <v>194833</v>
       </c>
       <c s="4" r="E11" t="n">
-        <v>196810</v>
+        <v>196866</v>
       </c>
       <c s="5" r="F11" t="n"/>
     </row>
@@ -2445,7 +2442,7 @@
         <v>38</v>
       </c>
       <c s="4" r="E14" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c s="5" r="F14" t="n"/>
       <c s="14" r="I14" t="n"/>
@@ -2459,7 +2456,7 @@
         <v>27</v>
       </c>
       <c s="4" r="E15" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c s="5" r="F15" t="n"/>
     </row>
@@ -2471,7 +2468,7 @@
         <v>134412</v>
       </c>
       <c s="4" r="E16" t="n">
-        <v>136690</v>
+        <v>136811</v>
       </c>
       <c s="5" r="F16" t="n"/>
     </row>
@@ -2484,7 +2481,7 @@
         <v/>
       </c>
       <c s="5" r="E17" t="n">
-        <v>0.9998</v>
+        <v>0.99981</v>
       </c>
       <c s="5" r="F17">
         <f>(E17-D17)/D17</f>
@@ -2538,7 +2535,7 @@
         <v>236021</v>
       </c>
       <c s="4" r="E21" t="n">
-        <v>286063</v>
+        <v>285733</v>
       </c>
       <c s="5" r="F21" t="n"/>
     </row>
@@ -2581,7 +2578,7 @@
         <v>7</v>
       </c>
       <c s="4" r="E24" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c s="5" r="F24" t="n"/>
     </row>
@@ -2593,7 +2590,7 @@
         <v>7</v>
       </c>
       <c s="4" r="E25" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c s="5" r="F25" t="n"/>
     </row>
@@ -2605,7 +2602,7 @@
         <v>553681</v>
       </c>
       <c s="4" r="E26" t="n">
-        <v>359154</v>
+        <v>392128</v>
       </c>
       <c s="5" r="F26" t="n"/>
     </row>
@@ -2672,7 +2669,7 @@
         <v>48710</v>
       </c>
       <c s="4" r="E31" t="n">
-        <v>55948</v>
+        <v>56505</v>
       </c>
       <c s="5" r="F31" t="n"/>
     </row>
@@ -2715,7 +2712,7 @@
         <v>463</v>
       </c>
       <c s="4" r="E34" t="n">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c s="5" r="F34" t="n"/>
     </row>
@@ -2727,7 +2724,7 @@
         <v>398</v>
       </c>
       <c s="4" r="E35" t="n">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c s="5" r="F35" t="n"/>
     </row>
@@ -2739,7 +2736,7 @@
         <v>187002</v>
       </c>
       <c s="4" r="E36" t="n">
-        <v>195669</v>
+        <v>200890</v>
       </c>
       <c s="5" r="F36" t="n"/>
     </row>
@@ -2752,7 +2749,7 @@
         <v/>
       </c>
       <c s="5" r="E37" t="n">
-        <v>0.99795</v>
+        <v>0.99802</v>
       </c>
       <c s="5" r="F37">
         <f>(E37-D37)/D37</f>
@@ -2782,7 +2779,7 @@
         <v>308</v>
       </c>
       <c s="4" r="E39" t="n">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c s="5" r="F39" t="n"/>
     </row>
@@ -2794,7 +2791,7 @@
         <v>257</v>
       </c>
       <c s="4" r="E40" t="n">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c s="5" r="F40" t="n"/>
     </row>
@@ -2806,7 +2803,7 @@
         <v>115443</v>
       </c>
       <c s="4" r="E41" t="n">
-        <v>120666</v>
+        <v>123444</v>
       </c>
       <c s="5" r="F41" t="n"/>
     </row>
@@ -2819,7 +2816,7 @@
         <v/>
       </c>
       <c s="5" r="E42" t="n">
-        <v>0.99775</v>
+        <v>0.99779</v>
       </c>
       <c s="5" r="F42">
         <f>(E42-D42)/D42</f>
@@ -2896,7 +2893,7 @@
         <v>32</v>
       </c>
       <c s="4" r="D3" t="n">
-        <v>5626</v>
+        <v>5799</v>
       </c>
       <c s="5" r="E3" t="n">
         <v>0.00497</v>
@@ -2908,10 +2905,10 @@
         <v>33</v>
       </c>
       <c s="6" r="H3" t="n">
-        <v>2673</v>
+        <v>2714</v>
       </c>
       <c s="5" r="I3" t="n">
-        <v>0.01358</v>
+        <v>0.01376</v>
       </c>
     </row>
     <row customHeight="1" r="4" ht="16.5" spans="1:9">
@@ -2922,10 +2919,10 @@
         <v>35</v>
       </c>
       <c s="4" r="D4" t="n">
-        <v>5057</v>
+        <v>5567</v>
       </c>
       <c s="5" r="E4" t="n">
-        <v>0.00446</v>
+        <v>0.00478</v>
       </c>
       <c s="2" r="F4" t="s">
         <v>34</v>
@@ -2934,10 +2931,10 @@
         <v>36</v>
       </c>
       <c s="6" r="H4" t="n">
-        <v>2491</v>
+        <v>2635</v>
       </c>
       <c s="5" r="I4" t="n">
-        <v>0.01265</v>
+        <v>0.01336</v>
       </c>
     </row>
     <row customHeight="1" r="5" ht="16.5" spans="1:9">
@@ -2948,10 +2945,10 @@
         <v>38</v>
       </c>
       <c s="4" r="D5" t="n">
-        <v>4764</v>
+        <v>5392</v>
       </c>
       <c s="5" r="E5" t="n">
-        <v>0.00421</v>
+        <v>0.00462</v>
       </c>
       <c s="2" r="F5" t="s">
         <v>37</v>
@@ -2960,10 +2957,10 @@
         <v>39</v>
       </c>
       <c s="6" r="H5" t="n">
-        <v>1075</v>
+        <v>937</v>
       </c>
       <c s="5" r="I5" t="n">
-        <v>0.00546</v>
+        <v>0.00475</v>
       </c>
     </row>
     <row customHeight="1" r="6" ht="16.5" spans="1:9">
@@ -2974,10 +2971,10 @@
         <v>41</v>
       </c>
       <c s="4" r="D6" t="n">
-        <v>1052</v>
+        <v>1223</v>
       </c>
       <c s="5" r="E6" t="n">
-        <v>0.0009300000000000001</v>
+        <v>0.00105</v>
       </c>
       <c s="2" r="F6" t="s">
         <v>40</v>
@@ -2986,10 +2983,10 @@
         <v>42</v>
       </c>
       <c s="6" r="H6" t="n">
-        <v>628</v>
+        <v>747</v>
       </c>
       <c s="5" r="I6" t="n">
-        <v>0.00319</v>
+        <v>0.00379</v>
       </c>
     </row>
     <row customHeight="1" r="7" ht="16.5" spans="1:9">
@@ -3000,10 +2997,10 @@
         <v>44</v>
       </c>
       <c s="4" r="D7" t="n">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c s="5" r="E7" t="n">
-        <v>0.0004</v>
+        <v>0.00038</v>
       </c>
       <c s="2" r="F7" t="s">
         <v>43</v>
@@ -3012,10 +3009,10 @@
         <v>45</v>
       </c>
       <c s="6" r="H7" t="n">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c s="5" r="I7" t="n">
-        <v>0.00315</v>
+        <v>0.00318</v>
       </c>
     </row>
     <row customHeight="1" r="8" ht="16.5" spans="1:9">
@@ -3026,10 +3023,10 @@
         <v>47</v>
       </c>
       <c s="4" r="D8" t="n">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c s="5" r="E8" t="n">
-        <v>0.00037</v>
+        <v>0.00036</v>
       </c>
       <c s="2" r="F8" t="s">
         <v>46</v>
@@ -3038,10 +3035,10 @@
         <v>48</v>
       </c>
       <c s="6" r="H8" t="n">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c s="5" r="I8" t="n">
-        <v>0.00312</v>
+        <v>0.00311</v>
       </c>
     </row>
     <row customHeight="1" r="9" ht="16.5" spans="1:9">
@@ -3052,10 +3049,10 @@
         <v>50</v>
       </c>
       <c s="4" r="D9" t="n">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c s="5" r="E9" t="n">
-        <v>0.00034</v>
+        <v>0.00033</v>
       </c>
       <c s="2" r="F9" t="s">
         <v>49</v>
@@ -3064,10 +3061,10 @@
         <v>51</v>
       </c>
       <c s="6" r="H9" t="n">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c s="5" r="I9" t="n">
-        <v>0.00287</v>
+        <v>0.00285</v>
       </c>
     </row>
     <row customHeight="1" r="10" ht="16.5" spans="1:9">
@@ -3078,10 +3075,10 @@
         <v>53</v>
       </c>
       <c s="4" r="D10" t="n">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c s="5" r="E10" t="n">
-        <v>0.00025</v>
+        <v>0.00024</v>
       </c>
       <c s="2" r="F10" t="s">
         <v>52</v>
@@ -3090,10 +3087,10 @@
         <v>54</v>
       </c>
       <c s="6" r="H10" t="n">
-        <v>522</v>
+        <v>540</v>
       </c>
       <c s="5" r="I10" t="n">
-        <v>0.00265</v>
+        <v>0.00274</v>
       </c>
     </row>
     <row customHeight="1" r="11" ht="16.5" spans="1:9">
@@ -3104,10 +3101,10 @@
         <v>56</v>
       </c>
       <c s="4" r="D11" t="n">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c s="5" r="E11" t="n">
-        <v>0.00019</v>
+        <v>0.0002</v>
       </c>
       <c s="2" r="F11" t="s">
         <v>55</v>
@@ -3116,10 +3113,10 @@
         <v>57</v>
       </c>
       <c s="6" r="H11" t="n">
-        <v>477</v>
+        <v>524</v>
       </c>
       <c s="5" r="I11" t="n">
-        <v>0.00242</v>
+        <v>0.00266</v>
       </c>
     </row>
     <row customHeight="1" r="12" ht="16.5" spans="1:9">
@@ -3130,10 +3127,10 @@
         <v>59</v>
       </c>
       <c s="4" r="D12" t="n">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c s="5" r="E12" t="n">
-        <v>0.00018</v>
+        <v>0.0002</v>
       </c>
       <c s="2" r="F12" t="s">
         <v>58</v>
@@ -3142,10 +3139,10 @@
         <v>60</v>
       </c>
       <c s="6" r="H12" t="n">
-        <v>253</v>
+        <v>274</v>
       </c>
       <c s="5" r="I12" t="n">
-        <v>0.00128</v>
+        <v>0.00139</v>
       </c>
     </row>
     <row customHeight="1" r="13" ht="16.5" spans="1:9">
@@ -3178,10 +3175,10 @@
         <v>36</v>
       </c>
       <c s="4" r="D14" t="n">
-        <v>1647</v>
+        <v>1711</v>
       </c>
       <c s="5" r="E14" t="n">
-        <v>0.012</v>
+        <v>0.01244</v>
       </c>
       <c s="2" r="F14" t="s">
         <v>31</v>
@@ -3190,10 +3187,10 @@
         <v>61</v>
       </c>
       <c s="6" r="H14" t="n">
-        <v>2144</v>
+        <v>2248</v>
       </c>
       <c s="5" r="I14" t="n">
-        <v>0.00368</v>
+        <v>0.00381</v>
       </c>
     </row>
     <row customHeight="1" r="15" ht="16.5" spans="1:9">
@@ -3204,10 +3201,10 @@
         <v>39</v>
       </c>
       <c s="4" r="D15" t="n">
-        <v>735</v>
+        <v>647</v>
       </c>
       <c s="5" r="E15" t="n">
-        <v>0.00535</v>
+        <v>0.0047</v>
       </c>
       <c s="2" r="F15" t="s">
         <v>34</v>
@@ -3216,10 +3213,10 @@
         <v>62</v>
       </c>
       <c s="6" r="H15" t="n">
-        <v>1399</v>
+        <v>1490</v>
       </c>
       <c s="5" r="I15" t="n">
-        <v>0.0024</v>
+        <v>0.00253</v>
       </c>
     </row>
     <row customHeight="1" r="16" ht="16.5" spans="1:9">
@@ -3227,13 +3224,13 @@
         <v>37</v>
       </c>
       <c s="3" r="C16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c s="4" r="D16" t="n">
-        <v>563</v>
+        <v>647</v>
       </c>
       <c s="5" r="E16" t="n">
-        <v>0.0041</v>
+        <v>0.0047</v>
       </c>
       <c s="2" r="F16" t="s">
         <v>37</v>
@@ -3242,10 +3239,10 @@
         <v>63</v>
       </c>
       <c s="6" r="H16" t="n">
-        <v>1273</v>
+        <v>1367</v>
       </c>
       <c s="5" r="I16" t="n">
-        <v>0.00219</v>
+        <v>0.00232</v>
       </c>
     </row>
     <row customHeight="1" r="17" ht="16.5" spans="1:9">
@@ -3253,13 +3250,13 @@
         <v>40</v>
       </c>
       <c s="3" r="C17" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c s="4" r="D17" t="n">
-        <v>560</v>
+        <v>593</v>
       </c>
       <c s="5" r="E17" t="n">
-        <v>0.00408</v>
+        <v>0.00431</v>
       </c>
       <c s="2" r="F17" t="s">
         <v>40</v>
@@ -3268,10 +3265,10 @@
         <v>64</v>
       </c>
       <c s="6" r="H17" t="n">
-        <v>520</v>
+        <v>535</v>
       </c>
       <c s="5" r="I17" t="n">
-        <v>0.0008899999999999999</v>
+        <v>0.00091</v>
       </c>
     </row>
     <row customHeight="1" r="18" ht="16.5" spans="1:9">
@@ -3279,13 +3276,13 @@
         <v>43</v>
       </c>
       <c s="3" r="C18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c s="4" r="D18" t="n">
-        <v>553</v>
+        <v>578</v>
       </c>
       <c s="5" r="E18" t="n">
-        <v>0.00403</v>
+        <v>0.0042</v>
       </c>
       <c s="2" r="F18" t="s">
         <v>43</v>
@@ -3294,10 +3291,10 @@
         <v>65</v>
       </c>
       <c s="6" r="H18" t="n">
-        <v>415</v>
+        <v>456</v>
       </c>
       <c s="5" r="I18" t="n">
-        <v>0.00071</v>
+        <v>0.00077</v>
       </c>
     </row>
     <row customHeight="1" r="19" ht="16.5" spans="1:9">
@@ -3308,10 +3305,10 @@
         <v>57</v>
       </c>
       <c s="4" r="D19" t="n">
-        <v>439</v>
+        <v>462</v>
       </c>
       <c s="5" r="E19" t="n">
-        <v>0.0032</v>
+        <v>0.00336</v>
       </c>
       <c s="2" r="F19" t="s">
         <v>46</v>
@@ -3320,10 +3317,10 @@
         <v>66</v>
       </c>
       <c s="6" r="H19" t="n">
-        <v>293</v>
+        <v>256</v>
       </c>
       <c s="5" r="I19" t="n">
-        <v>0.0005</v>
+        <v>0.00043</v>
       </c>
     </row>
     <row customHeight="1" r="20" ht="16.5" spans="1:9">
@@ -3334,10 +3331,10 @@
         <v>54</v>
       </c>
       <c s="4" r="D20" t="n">
-        <v>418</v>
+        <v>445</v>
       </c>
       <c s="5" r="E20" t="n">
-        <v>0.00305</v>
+        <v>0.00324</v>
       </c>
       <c s="2" r="F20" t="s">
         <v>49</v>
@@ -3346,10 +3343,10 @@
         <v>67</v>
       </c>
       <c s="6" r="H20" t="n">
-        <v>203</v>
+        <v>229</v>
       </c>
       <c s="5" r="I20" t="n">
-        <v>0.00035</v>
+        <v>0.00039</v>
       </c>
     </row>
     <row customHeight="1" r="21" ht="16.5" spans="1:9">
@@ -3357,25 +3354,25 @@
         <v>52</v>
       </c>
       <c s="3" r="C21" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c s="4" r="D21" t="n">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c s="5" r="E21" t="n">
-        <v>0.00154</v>
+        <v>0.00164</v>
       </c>
       <c s="2" r="F21" t="s">
         <v>52</v>
       </c>
       <c s="4" r="G21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c s="6" r="H21" t="n">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c s="5" r="I21" t="n">
-        <v>0.00034</v>
+        <v>0.00038</v>
       </c>
     </row>
     <row customHeight="1" r="22" ht="16.5" spans="1:9">
@@ -3383,13 +3380,13 @@
         <v>55</v>
       </c>
       <c s="3" r="C22" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c s="4" r="D22" t="n">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c s="5" r="E22" t="n">
-        <v>0.00136</v>
+        <v>0.00161</v>
       </c>
       <c s="2" r="F22" t="s">
         <v>55</v>
@@ -3398,10 +3395,10 @@
         <v>70</v>
       </c>
       <c s="6" r="H22" t="n">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c s="5" r="I22" t="n">
-        <v>0.00032</v>
+        <v>0.00036</v>
       </c>
     </row>
     <row customHeight="1" r="23" ht="16.5" spans="1:9">
@@ -3409,25 +3406,25 @@
         <v>58</v>
       </c>
       <c s="3" r="C23" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c s="4" r="D23" t="n">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c s="5" r="E23" t="n">
-        <v>0.00098</v>
+        <v>0.00102</v>
       </c>
       <c s="2" r="F23" t="s">
         <v>58</v>
       </c>
       <c s="4" r="G23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c s="6" r="H23" t="n">
-        <v>165</v>
+        <v>200</v>
       </c>
       <c s="5" r="I23" t="n">
-        <v>0.00028</v>
+        <v>0.00034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>